<commit_message>
test assets, test out gameflow (env. select, organism edit), some fixes
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5D7407-A4F0-4C79-87DD-5E35DA6FBA36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA95D3C2-FF61-4E4B-9A7B-D894B6CC36F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Key</t>
   </si>
@@ -44,6 +44,60 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>testBodyCapsule</t>
+  </si>
+  <si>
+    <t>Capsule</t>
+  </si>
+  <si>
+    <t>testBodySphere</t>
+  </si>
+  <si>
+    <t>Sphere</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Motility</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>categoryBody</t>
+  </si>
+  <si>
+    <t>categoryMotility</t>
+  </si>
+  <si>
+    <t>nucleoid</t>
+  </si>
+  <si>
+    <t>Nucleoid</t>
+  </si>
+  <si>
+    <t>ribosome</t>
+  </si>
+  <si>
+    <t>Ribosome</t>
   </si>
 </sst>
 </file>
@@ -376,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,6 +480,78 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
initial implement of binary fission, some stats stuff, initial categorization of archaea
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA95D3C2-FF61-4E4B-9A7B-D894B6CC36F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD139FB-BC99-4F78-9F82-9111258CD7AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4890" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Key</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t>Ribosome</t>
+  </si>
+  <si>
+    <t>categoryMetabolism</t>
+  </si>
+  <si>
+    <t>Metabolism</t>
+  </si>
+  <si>
+    <t>categoryCoating</t>
+  </si>
+  <si>
+    <t>Coating</t>
   </si>
 </sst>
 </file>
@@ -430,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,57 +510,73 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
setup energy and hazard sets, attribute info for display
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD139FB-BC99-4F78-9F82-9111258CD7AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E545C231-2C72-489D-986A-F3AC4EEED532}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Key</t>
   </si>
@@ -100,16 +100,34 @@
     <t>Ribosome</t>
   </si>
   <si>
-    <t>categoryMetabolism</t>
-  </si>
-  <si>
-    <t>Metabolism</t>
-  </si>
-  <si>
-    <t>categoryCoating</t>
-  </si>
-  <si>
-    <t>Coating</t>
+    <t>categoryCellStructure</t>
+  </si>
+  <si>
+    <t>Cell Structure</t>
+  </si>
+  <si>
+    <t>Thermophile</t>
+  </si>
+  <si>
+    <t>cellStructureThermophile</t>
+  </si>
+  <si>
+    <t>cellStructurePsychrophile</t>
+  </si>
+  <si>
+    <t>Psychrophile</t>
+  </si>
+  <si>
+    <t>cellStructureMethanogen</t>
+  </si>
+  <si>
+    <t>Methanogen</t>
+  </si>
+  <si>
+    <t>cellStructureHalophile</t>
+  </si>
+  <si>
+    <t>Halophile</t>
   </si>
 </sst>
 </file>
@@ -442,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,66 +536,90 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prep stuff for archaea, initial motility data
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E545C231-2C72-489D-986A-F3AC4EEED532}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6D57AF-8D42-49F5-BFBB-F332C3C3651B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5370" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Key</t>
   </si>
@@ -128,6 +128,30 @@
   </si>
   <si>
     <t>Halophile</t>
+  </si>
+  <si>
+    <t>motilityFlagellaMonotrichous</t>
+  </si>
+  <si>
+    <t>Monotrichous Flagella</t>
+  </si>
+  <si>
+    <t>motilityFlagellaLophotrichous</t>
+  </si>
+  <si>
+    <t>Lophotrichous Flagella</t>
+  </si>
+  <si>
+    <t>motilityFlagellaPeritrichous</t>
+  </si>
+  <si>
+    <t>Peritrichous Flagella</t>
+  </si>
+  <si>
+    <t>motilityFlagellaAmphitrichous</t>
+  </si>
+  <si>
+    <t>Amphitrichous Flagella</t>
   </si>
 </sst>
 </file>
@@ -460,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,6 +646,38 @@
         <v>35</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
added some of stage 1 parts, adjust physics logic
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6D57AF-8D42-49F5-BFBB-F332C3C3651B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E798DB3D-CE19-46C4-9A32-648011592B86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Key</t>
   </si>
@@ -152,6 +152,42 @@
   </si>
   <si>
     <t>Amphitrichous Flagella</t>
+  </si>
+  <si>
+    <t>bodyBacillus</t>
+  </si>
+  <si>
+    <t>Bacillus</t>
+  </si>
+  <si>
+    <t>bodyBacillusTiny</t>
+  </si>
+  <si>
+    <t>Tiny Bacillus</t>
+  </si>
+  <si>
+    <t>bodyCoccus</t>
+  </si>
+  <si>
+    <t>Coccus</t>
+  </si>
+  <si>
+    <t>bodyCoccobacillus</t>
+  </si>
+  <si>
+    <t>Coccobacillus</t>
+  </si>
+  <si>
+    <t>bodyCorkscrew</t>
+  </si>
+  <si>
+    <t>Corkscrew</t>
+  </si>
+  <si>
+    <t>bodyCoccusTiny</t>
+  </si>
+  <si>
+    <t>Tiny Coccus</t>
   </si>
 </sst>
 </file>
@@ -484,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,65 +652,113 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B27" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
body stuff for stage 1, some changes to energy (allow energy distribution to matching neighbor organisms)
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E798DB3D-CE19-46C4-9A32-648011592B86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F534FB50-2801-4039-81D1-336020E4C572}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4575" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Key</t>
   </si>
@@ -160,12 +160,6 @@
     <t>Bacillus</t>
   </si>
   <si>
-    <t>bodyBacillusTiny</t>
-  </si>
-  <si>
-    <t>Tiny Bacillus</t>
-  </si>
-  <si>
     <t>bodyCoccus</t>
   </si>
   <si>
@@ -182,12 +176,6 @@
   </si>
   <si>
     <t>Corkscrew</t>
-  </si>
-  <si>
-    <t>bodyCoccusTiny</t>
-  </si>
-  <si>
-    <t>Tiny Coccus</t>
   </si>
 </sst>
 </file>
@@ -520,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,89 +664,73 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
stage 2 prep, some rearrangement of data, organism spawner, energy spawner within organism.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F534FB50-2801-4039-81D1-336020E4C572}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B204327C-CCB3-4229-8053-7C4B2980355C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4575" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Key</t>
   </si>
@@ -88,15 +88,9 @@
     <t>categoryMotility</t>
   </si>
   <si>
-    <t>nucleoid</t>
-  </si>
-  <si>
     <t>Nucleoid</t>
   </si>
   <si>
-    <t>ribosome</t>
-  </si>
-  <si>
     <t>Ribosome</t>
   </si>
   <si>
@@ -172,10 +166,22 @@
     <t>Coccobacillus</t>
   </si>
   <si>
-    <t>bodyCorkscrew</t>
-  </si>
-  <si>
-    <t>Corkscrew</t>
+    <t>Plasmid DNA</t>
+  </si>
+  <si>
+    <t>essentialNucleoid</t>
+  </si>
+  <si>
+    <t>essentialRibosome</t>
+  </si>
+  <si>
+    <t>essentialPlasmid</t>
+  </si>
+  <si>
+    <t>Spirillum</t>
+  </si>
+  <si>
+    <t>bodySpirillum</t>
   </si>
 </sst>
 </file>
@@ -508,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,170 +574,178 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stage organism component setups, initial stage 2-1
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B204327C-CCB3-4229-8053-7C4B2980355C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97340580-13AB-474D-A761-F549F9307364}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4665" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Key</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Motility</t>
   </si>
   <si>
-    <t>Body</t>
-  </si>
-  <si>
     <t>categoryBody</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>categoryCellStructure</t>
   </si>
   <si>
-    <t>Cell Structure</t>
-  </si>
-  <si>
     <t>Thermophile</t>
   </si>
   <si>
@@ -182,6 +176,42 @@
   </si>
   <si>
     <t>bodySpirillum</t>
+  </si>
+  <si>
+    <t>categoryMetabolism</t>
+  </si>
+  <si>
+    <t>Metabolism</t>
+  </si>
+  <si>
+    <t>metabolismMethanotroph</t>
+  </si>
+  <si>
+    <t>Methanotroph</t>
+  </si>
+  <si>
+    <t>metabolismOrganotroph</t>
+  </si>
+  <si>
+    <t>Organotroph</t>
+  </si>
+  <si>
+    <t>metabolismEndobiotic</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>metabolismPhotoautotroph</t>
+  </si>
+  <si>
+    <t>Photoautotroph</t>
+  </si>
+  <si>
+    <t>Organotroph (Endobiotic)</t>
   </si>
 </sst>
 </file>
@@ -514,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,23 +636,23 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -630,122 +660,162 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ui art for dialog, options, confirm, hud stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97340580-13AB-474D-A761-F549F9307364}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25942B9-2203-4415-B742-EE48450A3CF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4665" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Key</t>
   </si>
@@ -43,9 +43,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>test1</t>
   </si>
   <si>
@@ -212,6 +209,63 @@
   </si>
   <si>
     <t>Organotroph (Endobiotic)</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>speech</t>
+  </si>
+  <si>
+    <t>SPEECH</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
+  </si>
+  <si>
+    <t>PERFECT CELL</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -544,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,231 +645,303 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more ui layouts and art.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25942B9-2203-4415-B742-EE48450A3CF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2B8191-BC89-4A37-8B87-B2C8CF0D4DBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4665" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Key</t>
   </si>
@@ -199,9 +199,6 @@
     <t>Structure</t>
   </si>
   <si>
-    <t>Shape</t>
-  </si>
-  <si>
     <t>metabolismPhotoautotroph</t>
   </si>
   <si>
@@ -266,6 +263,63 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>BACK</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>OKAY</t>
+  </si>
+  <si>
+    <t>retry</t>
+  </si>
+  <si>
+    <t>RETRY</t>
+  </si>
+  <si>
+    <t>changeEnvironment</t>
+  </si>
+  <si>
+    <t>CHANGE ENVIRONMENT</t>
+  </si>
+  <si>
+    <t>editOrganism</t>
+  </si>
+  <si>
+    <t>EDIT ORGANISM</t>
+  </si>
+  <si>
+    <t>timeExpire</t>
+  </si>
+  <si>
+    <t>Time's Up</t>
+  </si>
+  <si>
+    <t>timeExpireDesc</t>
+  </si>
+  <si>
+    <t>You only got {0} out of {1} organisms.</t>
   </si>
 </sst>
 </file>
@@ -598,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +699,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,274 +728,346 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
         <v>63</v>
-      </c>
-      <c r="B7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
         <v>65</v>
-      </c>
-      <c r="B8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
         <v>67</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
         <v>69</v>
-      </c>
-      <c r="B10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
         <v>71</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
         <v>73</v>
-      </c>
-      <c r="B12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
         <v>75</v>
-      </c>
-      <c r="B13" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
         <v>78</v>
-      </c>
-      <c r="B14" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
         <v>80</v>
-      </c>
-      <c r="B15" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>57</v>
       </c>
-      <c r="B40" t="s">
-        <v>62</v>
+      <c r="B49" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
environment details and ui stuff, some bug fixes
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41763101-7B5F-42D8-80A8-E7D50F04B26E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD53DF1-E2E8-4379-81C4-A688699CB36D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4665" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="179">
   <si>
     <t>Key</t>
   </si>
@@ -344,6 +344,219 @@
   </si>
   <si>
     <t>Score:</t>
+  </si>
+  <si>
+    <t>stage_1_1_title</t>
+  </si>
+  <si>
+    <t>stage_1_1_desc</t>
+  </si>
+  <si>
+    <t>stage_1_2_title</t>
+  </si>
+  <si>
+    <t>stage_1_2_desc</t>
+  </si>
+  <si>
+    <t>stage_1_3_title</t>
+  </si>
+  <si>
+    <t>stage_1_3_desc</t>
+  </si>
+  <si>
+    <t>stage_2_1_title</t>
+  </si>
+  <si>
+    <t>stage_2_1_desc</t>
+  </si>
+  <si>
+    <t>stage_2_2_title</t>
+  </si>
+  <si>
+    <t>stage_2_2_desc</t>
+  </si>
+  <si>
+    <t>stage_2_3_title</t>
+  </si>
+  <si>
+    <t>stage_2_3_desc</t>
+  </si>
+  <si>
+    <t>stage_3_1_title</t>
+  </si>
+  <si>
+    <t>stage_3_1_desc</t>
+  </si>
+  <si>
+    <t>stage_3_2_title</t>
+  </si>
+  <si>
+    <t>stage_3_2_desc</t>
+  </si>
+  <si>
+    <t>stage_3_3_title</t>
+  </si>
+  <si>
+    <t>stage_3_3_desc</t>
+  </si>
+  <si>
+    <t>Hydrothermal Vent</t>
+  </si>
+  <si>
+    <t>A fissure found on the seafloor near volcanically active places. Temperature can reach as high as 867 °F.</t>
+  </si>
+  <si>
+    <t>Colon</t>
+  </si>
+  <si>
+    <t>The last part of the digestive tract found inside animals. This is where the remaining materials are broken down with the help of bacteria and archaea before excretion.</t>
+  </si>
+  <si>
+    <t>Red Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A seawater inlet located between Africa and Asia. The Red Sea is one of the saltiest waters in the world, a perfect place for salt-loving creatures. </t>
+  </si>
+  <si>
+    <t>Septic Water</t>
+  </si>
+  <si>
+    <t>The kind of water found in sewer where all the wastes accumulate. A perfect home for all sorts of bacteria.</t>
+  </si>
+  <si>
+    <t>Pond</t>
+  </si>
+  <si>
+    <t>Known as the windpipe that connects the larynx, and the bronchi of the lungs. Many foreign organisms are disposed of here by the hands of white blood cells. Beware of the wandering macrophages.</t>
+  </si>
+  <si>
+    <t>Trachea</t>
+  </si>
+  <si>
+    <t>Murky Swamp</t>
+  </si>
+  <si>
+    <t>A body of freshwater filled with grime. This particular area is filled with toxic bacteria, not ideal for consumption.</t>
+  </si>
+  <si>
+    <t>Whirlpool</t>
+  </si>
+  <si>
+    <t>A body of freshwater within a land brimming with life. Where there are thriving populations of organisms, so too, will there be predators.</t>
+  </si>
+  <si>
+    <t>A body of freshwater within a land brimming with life. A perfect place for predatory organisms.</t>
+  </si>
+  <si>
+    <t>Watch out for this downward spiral into the void. However, with this many organisms being pulled in, it’s sure to be a buffet.</t>
+  </si>
+  <si>
+    <t>attributeCategoryHazards</t>
+  </si>
+  <si>
+    <t>Hazards</t>
+  </si>
+  <si>
+    <t>attributeCategoryEnergy</t>
+  </si>
+  <si>
+    <t>Energy Sources</t>
+  </si>
+  <si>
+    <t>attributeHazardExtremeHighTemperature</t>
+  </si>
+  <si>
+    <t>attributeHazardHighSalinity</t>
+  </si>
+  <si>
+    <t>High Salinity</t>
+  </si>
+  <si>
+    <t>attributeHazardUVRadiation</t>
+  </si>
+  <si>
+    <t>UV Radiation</t>
+  </si>
+  <si>
+    <t>energySulfur</t>
+  </si>
+  <si>
+    <t>Sulfur</t>
+  </si>
+  <si>
+    <t>energyH2</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>energyAminoAcid</t>
+  </si>
+  <si>
+    <t>Amino Acid</t>
+  </si>
+  <si>
+    <t>Sunlight</t>
+  </si>
+  <si>
+    <t>energySunlight</t>
+  </si>
+  <si>
+    <t>attributeHazardHighMethane</t>
+  </si>
+  <si>
+    <t>Methane</t>
+  </si>
+  <si>
+    <t>attributeHazardLowOxygen</t>
+  </si>
+  <si>
+    <t>Low Oxygen</t>
+  </si>
+  <si>
+    <t>energyMethane</t>
+  </si>
+  <si>
+    <t>energyGlucose</t>
+  </si>
+  <si>
+    <t>Glucose</t>
+  </si>
+  <si>
+    <t>attributeCategoryDanger</t>
+  </si>
+  <si>
+    <t>Danger</t>
+  </si>
+  <si>
+    <t>attributeDangerHunter</t>
+  </si>
+  <si>
+    <t>attributeDangerMacrophage</t>
+  </si>
+  <si>
+    <t>Macrophage</t>
+  </si>
+  <si>
+    <t>attributeDangerNeutrophil</t>
+  </si>
+  <si>
+    <t>Neutrophil</t>
+  </si>
+  <si>
+    <t>Stentor</t>
+  </si>
+  <si>
+    <t>attributeDangerToxic</t>
+  </si>
+  <si>
+    <t>Toxic Bacteria</t>
+  </si>
+  <si>
+    <t>attributeDangerWhirlpool</t>
+  </si>
+  <si>
+    <t>Extreme Heat</t>
   </si>
 </sst>
 </file>
@@ -393,9 +606,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,6 +1342,302 @@
         <v>61</v>
       </c>
     </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>116</v>
+      </c>
+      <c r="B62" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>119</v>
+      </c>
+      <c r="B65" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>121</v>
+      </c>
+      <c r="B67" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>122</v>
+      </c>
+      <c r="B68" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>123</v>
+      </c>
+      <c r="B69" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>124</v>
+      </c>
+      <c r="B70" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>125</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>152</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>154</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>156</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>159</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>164</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>165</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>143</v>
+      </c>
+      <c r="B78" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>167</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>147</v>
+      </c>
+      <c r="B81" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>148</v>
+      </c>
+      <c r="B82" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>150</v>
+      </c>
+      <c r="B83" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>160</v>
+      </c>
+      <c r="B84" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>162</v>
+      </c>
+      <c r="B85" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>170</v>
+      </c>
+      <c r="B87" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>177</v>
+      </c>
+      <c r="B90" t="s">
+        <v>139</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
bunch of fixes and refactor in edit mode, most art and description in edit mode
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD53DF1-E2E8-4379-81C4-A688699CB36D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CA1CEF-FCB3-448E-8EB7-966BBC47823C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="3195" windowWidth="19065" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="225">
   <si>
     <t>Key</t>
   </si>
@@ -205,9 +205,6 @@
     <t>Photoautotroph</t>
   </si>
   <si>
-    <t>Organotroph (Endobiotic)</t>
-  </si>
-  <si>
     <t>options</t>
   </si>
   <si>
@@ -526,9 +523,6 @@
     <t>attributeCategoryDanger</t>
   </si>
   <si>
-    <t>Danger</t>
-  </si>
-  <si>
     <t>attributeDangerHunter</t>
   </si>
   <si>
@@ -557,6 +551,150 @@
   </si>
   <si>
     <t>Extreme Heat</t>
+  </si>
+  <si>
+    <t>confirmPlayExitTitle</t>
+  </si>
+  <si>
+    <t>confirmPlayExitDesc</t>
+  </si>
+  <si>
+    <t>EXIT SIMULATION</t>
+  </si>
+  <si>
+    <t>Are you sure you want to exit the simulation?</t>
+  </si>
+  <si>
+    <t>essentialNucleoidDesc</t>
+  </si>
+  <si>
+    <t>Contains the genetic information of the prokaryotic cell. The nucleoid determines how the cell will develop and grow.</t>
+  </si>
+  <si>
+    <t>essentialRibosomeDesc</t>
+  </si>
+  <si>
+    <t>essentialPlasmidDesc</t>
+  </si>
+  <si>
+    <t>These are extra DNA molecules that are commonly found in bacteria, and sometimes in other cells. They allow cells to mutate and adapt to an ever-changing environment.</t>
+  </si>
+  <si>
+    <t>Responsible for making proteins. These proteins are what keeps the cell alive by providing energy for movement, repair, and growth.</t>
+  </si>
+  <si>
+    <t>cellStructureThermophileDesc</t>
+  </si>
+  <si>
+    <t>An affinity for extremely hot temperature. These archaeans can thrive in environments near volcanos, hot springs, and acidic soils.</t>
+  </si>
+  <si>
+    <t>cellStructureMethanogenDesc</t>
+  </si>
+  <si>
+    <t>These archaeans release methane as a result of digesting materials such as carbon and hydrogen. They are known to play a role in breaking up materials for other cells to consume.</t>
+  </si>
+  <si>
+    <t>cellStructureHalophileDesc</t>
+  </si>
+  <si>
+    <t>An affinity for salt. These archaeans can withstand the effects of salt which causes dehydration. They are also known to be resistant to UV radiation, giving them a reddish look.</t>
+  </si>
+  <si>
+    <t>motilityFlagellaMonotrichousDesc</t>
+  </si>
+  <si>
+    <t>motilityFlagellaLophotrichousDesc</t>
+  </si>
+  <si>
+    <t>A single flagellum that favors long distance travel.</t>
+  </si>
+  <si>
+    <t>Multiple flagella in one polar end of the cell that favors frequent twists and turns.</t>
+  </si>
+  <si>
+    <t>Multiple flagella around the cell that helps with even more frequent twists and turns.</t>
+  </si>
+  <si>
+    <t>motilityFlagellaPeritrichousDesc</t>
+  </si>
+  <si>
+    <t>motilityFlagellaAmphitrichousDesc</t>
+  </si>
+  <si>
+    <t>A flagellum on two polar opposites of the cell.</t>
+  </si>
+  <si>
+    <t>attributeCategoryResistance</t>
+  </si>
+  <si>
+    <t>Resistances</t>
+  </si>
+  <si>
+    <t>Dangers</t>
+  </si>
+  <si>
+    <t>attributeCategoryConsumes</t>
+  </si>
+  <si>
+    <t>Consumes</t>
+  </si>
+  <si>
+    <t>stageTitle_1</t>
+  </si>
+  <si>
+    <t>Archaea</t>
+  </si>
+  <si>
+    <t>stageTitle_2</t>
+  </si>
+  <si>
+    <t>Bacteria</t>
+  </si>
+  <si>
+    <t>stageTitle_3</t>
+  </si>
+  <si>
+    <t>Protozoa</t>
+  </si>
+  <si>
+    <t>attributeResistanceAnaerobic</t>
+  </si>
+  <si>
+    <t>Anaerobic</t>
+  </si>
+  <si>
+    <t>Antiphagocytic</t>
+  </si>
+  <si>
+    <t>attributeResistanceAntiphagocytic</t>
+  </si>
+  <si>
+    <t>Endobiotic Parasite</t>
+  </si>
+  <si>
+    <t>metabolismMethanotrophDesc</t>
+  </si>
+  <si>
+    <t>A prokaryote that metabolizes methane. This particular type is anaerobic, which means it can live with little to no oxygen.</t>
+  </si>
+  <si>
+    <t>metabolismPhotoautotrophDesc</t>
+  </si>
+  <si>
+    <t>Capable of harnessing energy from sunlight to produce food from inorganic matter. Its chlorophyl component gives it a green color.</t>
+  </si>
+  <si>
+    <t>metabolismOrganotrophDesc</t>
+  </si>
+  <si>
+    <t>Eats anything organic that contains carbon and hydrogen, such as glucose.</t>
+  </si>
+  <si>
+    <t>metabolismEndobioticDesc</t>
+  </si>
+  <si>
+    <t>This particular bacteria feeds from within the host, draining it of all its energy. Once engulfed, it secretes special proteins that will prevent itself from being consumed.</t>
   </si>
 </sst>
 </file>
@@ -892,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,7 +1077,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -968,178 +1106,178 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
         <v>62</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
         <v>64</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
         <v>66</v>
-      </c>
-      <c r="B9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
         <v>68</v>
-      </c>
-      <c r="B10" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
         <v>70</v>
-      </c>
-      <c r="B11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
         <v>72</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
         <v>74</v>
-      </c>
-      <c r="B13" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
         <v>77</v>
-      </c>
-      <c r="B14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
         <v>79</v>
-      </c>
-      <c r="B15" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
         <v>88</v>
-      </c>
-      <c r="B16" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
         <v>81</v>
-      </c>
-      <c r="B17" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
         <v>83</v>
-      </c>
-      <c r="B18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" t="s">
         <v>85</v>
-      </c>
-      <c r="B19" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
         <v>96</v>
-      </c>
-      <c r="B20" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
         <v>98</v>
-      </c>
-      <c r="B21" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" t="s">
         <v>90</v>
-      </c>
-      <c r="B22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
         <v>100</v>
-      </c>
-      <c r="B23" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" t="s">
         <v>102</v>
-      </c>
-      <c r="B24" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" t="s">
         <v>106</v>
-      </c>
-      <c r="B26" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
         <v>92</v>
-      </c>
-      <c r="B27" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
         <v>94</v>
-      </c>
-      <c r="B28" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1160,482 +1298,750 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>206</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>208</v>
+      </c>
+      <c r="B32" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>210</v>
+      </c>
+      <c r="B33" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>22</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B35" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>19</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>46</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>181</v>
+      </c>
+      <c r="B39" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>47</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>48</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B42" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C42">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>184</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>39</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>41</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>43</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>50</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B47" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>24</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B48" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="C48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>187</v>
+      </c>
+      <c r="B49" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>25</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B50" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>27</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B51" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="C51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>189</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>29</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B53" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="C53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>31</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B55" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="C55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>193</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>33</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B57" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="C57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>35</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B59" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="C59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>198</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>37</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B61" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="C61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>199</v>
+      </c>
+      <c r="B62" t="s">
+        <v>200</v>
+      </c>
+      <c r="C62">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>53</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B63" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="C63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>217</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C64">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>59</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B65" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="C65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>219</v>
+      </c>
+      <c r="B66" t="s">
+        <v>220</v>
+      </c>
+      <c r="C66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>55</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B67" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="C67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>221</v>
+      </c>
+      <c r="B68" t="s">
+        <v>222</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>57</v>
       </c>
-      <c r="B53" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B69" t="s">
+        <v>216</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>223</v>
+      </c>
+      <c r="B70" t="s">
+        <v>224</v>
+      </c>
+      <c r="C70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>107</v>
+      </c>
+      <c r="B71" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>108</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B72" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>109</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B73" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>110</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B74" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B75" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>112</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B76" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>113</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B77" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>114</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B78" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>115</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B79" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>116</v>
       </c>
-      <c r="B62" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>117</v>
-      </c>
-      <c r="B63" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>118</v>
-      </c>
-      <c r="B64" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>119</v>
-      </c>
-      <c r="B65" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>120</v>
-      </c>
-      <c r="B66" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>121</v>
-      </c>
-      <c r="B67" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>122</v>
-      </c>
-      <c r="B68" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>123</v>
-      </c>
-      <c r="B69" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>124</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="B80" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>125</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>152</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>154</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>156</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>159</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>164</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>165</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>143</v>
-      </c>
-      <c r="B78" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>145</v>
-      </c>
-      <c r="B79" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>167</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="B81" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="B82" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="B83" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="B84" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="B85" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="B86" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="B87" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>172</v>
-      </c>
-      <c r="B88" t="s">
-        <v>173</v>
+        <v>124</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>175</v>
-      </c>
-      <c r="B89" t="s">
-        <v>176</v>
+        <v>151</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>153</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>158</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>163</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>164</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>142</v>
+      </c>
+      <c r="B95" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>144</v>
+      </c>
+      <c r="B96" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>166</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>201</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>204</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>146</v>
+      </c>
+      <c r="B100" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>147</v>
+      </c>
+      <c r="B101" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>149</v>
+      </c>
+      <c r="B102" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>159</v>
+      </c>
+      <c r="B103" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>161</v>
+      </c>
+      <c r="B104" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>167</v>
+      </c>
+      <c r="B105" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>168</v>
+      </c>
+      <c r="B106" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>170</v>
+      </c>
+      <c r="B107" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>173</v>
+      </c>
+      <c r="B108" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>175</v>
+      </c>
+      <c r="B109" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>212</v>
+      </c>
+      <c r="B110" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>215</v>
+      </c>
+      <c r="B111" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>177</v>
       </c>
-      <c r="B90" t="s">
-        <v>139</v>
+      <c r="B112" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>178</v>
+      </c>
+      <c r="B113" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
intro 1 and 2, tutorials
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855BF98B-58EF-4AEB-A6C0-20FB5C601011}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F0EC7A-5714-48A3-ACC2-BD2E973C3D94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6555" yWindow="3495" windowWidth="19065" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="2595" windowWidth="19065" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="382">
   <si>
     <t>Key</t>
   </si>
@@ -580,9 +580,6 @@
     <t>These are extra DNA molecules that are commonly found in bacteria, and sometimes in other cells. They allow cells to mutate and adapt to an ever-changing environment.</t>
   </si>
   <si>
-    <t>Responsible for making proteins. These proteins are what keeps the cell alive by providing energy for movement, repair, and growth.</t>
-  </si>
-  <si>
     <t>cellStructureThermophileDesc</t>
   </si>
   <si>
@@ -845,6 +842,330 @@
   </si>
   <si>
     <t>There is already a game in progress. Are you sure you want to start a new game?</t>
+  </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>Written By: David Dionisio</t>
+  </si>
+  <si>
+    <t>hint_1_1</t>
+  </si>
+  <si>
+    <t>hint_1_2</t>
+  </si>
+  <si>
+    <t>hint_1_3</t>
+  </si>
+  <si>
+    <t>hint_2_1</t>
+  </si>
+  <si>
+    <t>hint_2_2</t>
+  </si>
+  <si>
+    <t>hint_2_3</t>
+  </si>
+  <si>
+    <t>hint_3_1</t>
+  </si>
+  <si>
+    <t>hint_3_2</t>
+  </si>
+  <si>
+    <t>hint_3_3</t>
+  </si>
+  <si>
+    <t>This environment is mostly filled with hydrogen components. An organism capable of digesting such materials will do well here.</t>
+  </si>
+  <si>
+    <t>This environment contains high concentration of salt, along with UV radiation. Unless an organism can withstand both salt and UV radiation, it will dry up to death.</t>
+  </si>
+  <si>
+    <t>This environment is low on oxygen, and filled with methane. Only an anaerobic, methane-eating bacterial will do well here.</t>
+  </si>
+  <si>
+    <t>If you are having difficulty with these predators, perhaps deploying parasitic bacteria will do the trick. Otherwise, this environment mostly provides glucose and sunlight.</t>
+  </si>
+  <si>
+    <t>Most bacteria cannot stand a chance against white blood cells, unless they are completely overwhelmed. For a greater success, try deploying parasitic bacteria.</t>
+  </si>
+  <si>
+    <t>This environment has a mixture of big and small organisms. A predator capable of hunting both will benefit the most here.</t>
+  </si>
+  <si>
+    <t>Toxic bacteria dominate this environment. An organism that can resist toxins should be able to thrive here.</t>
+  </si>
+  <si>
+    <t>The whirlpool is a pain, try to deploy your organisms at the outer region. That aside, an organism with strong propellant should be able to maneuver around it with much ease.</t>
+  </si>
+  <si>
+    <t>This environment is extremely hot! Only an organism capable of resisting the heat will be able to thrive here.</t>
+  </si>
+  <si>
+    <t>Responsible for making proteins. These proteins are the workers of the cell, they provide energy for communication, repair, and growth.</t>
+  </si>
+  <si>
+    <t>cellClassification</t>
+  </si>
+  <si>
+    <t>CELL CLASSIFICATION</t>
+  </si>
+  <si>
+    <t>organism</t>
+  </si>
+  <si>
+    <t>Organism</t>
+  </si>
+  <si>
+    <t>prokaryote</t>
+  </si>
+  <si>
+    <t>Prokaryote</t>
+  </si>
+  <si>
+    <t>singleCellular</t>
+  </si>
+  <si>
+    <t>Single Cellular</t>
+  </si>
+  <si>
+    <t>archaea</t>
+  </si>
+  <si>
+    <t>bacteria</t>
+  </si>
+  <si>
+    <t>eukaryote</t>
+  </si>
+  <si>
+    <t>Eukaryote</t>
+  </si>
+  <si>
+    <t>multiCellular</t>
+  </si>
+  <si>
+    <t>Multicellular</t>
+  </si>
+  <si>
+    <t>protist</t>
+  </si>
+  <si>
+    <t>Protist</t>
+  </si>
+  <si>
+    <t>multiCellularEtc</t>
+  </si>
+  <si>
+    <t>Fungi, Plants, Animals</t>
+  </si>
+  <si>
+    <t>intro01_intro0</t>
+  </si>
+  <si>
+    <t>intro01_intro1</t>
+  </si>
+  <si>
+    <t>intro01_intro2</t>
+  </si>
+  <si>
+    <t>intro01_intro3</t>
+  </si>
+  <si>
+    <t>I am here to guide you on this journey to learn about cells.</t>
+  </si>
+  <si>
+    <t>But not just any cell…</t>
+  </si>
+  <si>
+    <t>The perfect cell!</t>
+  </si>
+  <si>
+    <t>intro01_spec0</t>
+  </si>
+  <si>
+    <t>intro01_blob0</t>
+  </si>
+  <si>
+    <t>intro01_blob1</t>
+  </si>
+  <si>
+    <t>intro01_classification0</t>
+  </si>
+  <si>
+    <t>intro01_classification1</t>
+  </si>
+  <si>
+    <t>intro01_blob2</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_environment0</t>
+  </si>
+  <si>
+    <t>We will begin our journey as archeans, the extremophiles of the prokaryote cells!</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_environment1</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_environment2</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_edit0</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_edit1</t>
+  </si>
+  <si>
+    <t>plasmaMembrane</t>
+  </si>
+  <si>
+    <t>Plasma Membrane</t>
+  </si>
+  <si>
+    <t>cytoplasm</t>
+  </si>
+  <si>
+    <t>Cytoplasm</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_body0</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_membrane0</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_cytoplasm0</t>
+  </si>
+  <si>
+    <t>Cytoplasm is the fluid that fills the cell. Its role is to sustain the structure and flow within the cell, along with metabolic activity.</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_bodyEnd0</t>
+  </si>
+  <si>
+    <t>Press the left and right arrow on the side of the screen to switch between environments. Keep in mind the hazards and energy sources!</t>
+  </si>
+  <si>
+    <t>Once you’ve decided, press the button on the lower right of the screen to proceed.</t>
+  </si>
+  <si>
+    <t>Now it’s time to shape the perfect cell!</t>
+  </si>
+  <si>
+    <t>Although organisms go through evolution in order to shape itself, you will instead choose what’s best.</t>
+  </si>
+  <si>
+    <t>The plasma membrane is a barrier that determines what goes in and out of the cell. That is something we can decide later.</t>
+  </si>
+  <si>
+    <t>Now you will place the internal components that keeps the cell alive.</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_essenceComplete0</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_essenceComplete1</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_essenceComplete2</t>
+  </si>
+  <si>
+    <t>Excellent! With all the essentials of the cells filled, we can now choose the other components.</t>
+  </si>
+  <si>
+    <t>In order for the cell to survive, pick the right structure that determines its resistance and energy source.</t>
+  </si>
+  <si>
+    <t>A cell cannot reach its energy source efficiently without proper motility. Pick a form of motility to determine how the cell moves.</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_play0</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_play1</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_play2</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_play3</t>
+  </si>
+  <si>
+    <t>You can find the population number, and the progress at the bottom left of the screen.</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_time_forward</t>
+  </si>
+  <si>
+    <t>tutorial_stage01_victory</t>
+  </si>
+  <si>
+    <t>Press this button to speed things up!</t>
+  </si>
+  <si>
+    <t>Before we continue, let’s take a moment to look at the two components that keep the cell together.</t>
+  </si>
+  <si>
+    <t>Here we are going to choose which environment our organisms are going to inhabit.</t>
+  </si>
+  <si>
+    <t>To deploy an organism, press any valid location on the screen. You have a limited amount to deploy, so choose each location wisely.</t>
+  </si>
+  <si>
+    <t>Time is limited, and when it is reached, all is lost. This is displayed at the bottom of the screen.</t>
+  </si>
+  <si>
+    <t>Now that we’re here, the goal is to grow the population of our organisms to a certain amount.</t>
+  </si>
+  <si>
+    <t>Good work! Now let’s try another environment, and then we can move on to grander things!</t>
+  </si>
+  <si>
+    <t>In this vast sea of nothingness comes a lifeless inorganic spec.</t>
+  </si>
+  <si>
+    <t>By mysterious circumstances, various chemicals have gathered and formed to create a living organism.</t>
+  </si>
+  <si>
+    <t>In order to maintain its form, it must continuously consume materials, and convert them to energy.</t>
+  </si>
+  <si>
+    <t>But it can only maintain its form for so long…with your help however, we can let it grow, and reproduce for many generations!</t>
+  </si>
+  <si>
+    <t>intro02_intro0</t>
+  </si>
+  <si>
+    <t>This is the classification of cells. As you can see, a cell can be one of two things: Prokaryote or Eukaryote.</t>
+  </si>
+  <si>
+    <t>intro02_intro1</t>
+  </si>
+  <si>
+    <t>As the perfect cells pass through numerous environments, few are able to adapt.</t>
+  </si>
+  <si>
+    <t>A new strategy for adaptation is in order.</t>
+  </si>
+  <si>
+    <t>intro02_classification0</t>
+  </si>
+  <si>
+    <t>intro02_classification1</t>
+  </si>
+  <si>
+    <t>intro02_classification2</t>
+  </si>
+  <si>
+    <t>We will now be moving forward as bacteria.</t>
+  </si>
+  <si>
+    <t>Though they are structurally similar to archaea, they differ in how their membrane is structured.</t>
+  </si>
+  <si>
+    <t>Now let’s see how they fare with the next environments!</t>
   </si>
 </sst>
 </file>
@@ -1180,10 +1501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D138"/>
+  <dimension ref="A1:D193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,1093 +1553,1093 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>274</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>271</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>270</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>206</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>207</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B33" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B34" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>209</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>181</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>182</v>
+        <v>20</v>
       </c>
       <c r="C40">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>181</v>
       </c>
       <c r="B41" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>183</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>186</v>
+        <v>21</v>
       </c>
       <c r="C42">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>183</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>294</v>
       </c>
       <c r="C43">
-        <v>2.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>184</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>185</v>
+        <v>48</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
       </c>
       <c r="C44">
-        <v>8</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>229</v>
+        <v>184</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="C45">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>231</v>
-      </c>
-      <c r="B46" t="s">
-        <v>244</v>
+        <v>228</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>232</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
+      </c>
+      <c r="B47" t="s">
+        <v>243</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="C48">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>237</v>
-      </c>
-      <c r="B50" t="s">
-        <v>246</v>
+        <v>234</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="C50">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>238</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
+      </c>
+      <c r="B51" t="s">
+        <v>245</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C52">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C53">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>243</v>
-      </c>
-      <c r="B54" t="s">
-        <v>248</v>
+        <v>240</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="C54">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>242</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>247</v>
+      </c>
+      <c r="C55">
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>249</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>250</v>
-      </c>
-      <c r="C59">
-        <v>2</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B60" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C60">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B61" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>252</v>
+      </c>
+      <c r="B62" t="s">
         <v>254</v>
       </c>
-      <c r="B62" t="s">
-        <v>256</v>
-      </c>
       <c r="C62">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B63" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>257</v>
-      </c>
-      <c r="B64" s="2" t="s">
         <v>258</v>
       </c>
+      <c r="B64" t="s">
+        <v>259</v>
+      </c>
       <c r="C64">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>24</v>
-      </c>
-      <c r="B65" t="s">
-        <v>23</v>
+        <v>256</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>187</v>
+        <v>24</v>
       </c>
       <c r="B66" t="s">
-        <v>188</v>
+        <v>23</v>
       </c>
       <c r="C66">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>186</v>
       </c>
       <c r="B67" t="s">
-        <v>26</v>
+        <v>187</v>
+      </c>
+      <c r="C67">
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
-      </c>
-      <c r="C68">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>189</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>190</v>
+        <v>27</v>
+      </c>
+      <c r="B69" t="s">
+        <v>28</v>
       </c>
       <c r="C69">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>29</v>
-      </c>
-      <c r="B70" t="s">
-        <v>30</v>
+        <v>188</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="C70">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>191</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>192</v>
+        <v>29</v>
+      </c>
+      <c r="B71" t="s">
+        <v>30</v>
       </c>
       <c r="C71">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>31</v>
-      </c>
-      <c r="B72" t="s">
-        <v>32</v>
+        <v>190</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>193</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>195</v>
+        <v>31</v>
+      </c>
+      <c r="B73" t="s">
+        <v>32</v>
       </c>
       <c r="C73">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>33</v>
-      </c>
-      <c r="B74" t="s">
-        <v>34</v>
+        <v>192</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>194</v>
+        <v>33</v>
       </c>
       <c r="B75" t="s">
-        <v>196</v>
+        <v>34</v>
       </c>
       <c r="C75">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>35</v>
+        <v>193</v>
       </c>
       <c r="B76" t="s">
-        <v>36</v>
+        <v>195</v>
       </c>
       <c r="C76">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>198</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>197</v>
+        <v>35</v>
+      </c>
+      <c r="B77" t="s">
+        <v>36</v>
       </c>
       <c r="C77">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>37</v>
-      </c>
-      <c r="B78" t="s">
-        <v>38</v>
+        <v>197</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>199</v>
+        <v>37</v>
       </c>
       <c r="B79" t="s">
-        <v>200</v>
+        <v>38</v>
       </c>
       <c r="C79">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="B80" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B81" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C81">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="B82" t="s">
-        <v>265</v>
+        <v>226</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B83" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C83">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B84" t="s">
         <v>266</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B85" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C85">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>53</v>
+        <v>263</v>
       </c>
       <c r="B86" t="s">
-        <v>54</v>
+        <v>267</v>
       </c>
       <c r="C86">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>217</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>218</v>
+        <v>53</v>
+      </c>
+      <c r="B87" t="s">
+        <v>54</v>
       </c>
       <c r="C87">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>59</v>
-      </c>
-      <c r="B88" t="s">
-        <v>60</v>
+        <v>216</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>219</v>
+        <v>59</v>
       </c>
       <c r="B89" t="s">
-        <v>228</v>
+        <v>60</v>
       </c>
       <c r="C89">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>55</v>
+        <v>218</v>
       </c>
       <c r="B90" t="s">
-        <v>56</v>
+        <v>227</v>
       </c>
       <c r="C90">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>220</v>
+        <v>55</v>
       </c>
       <c r="B91" t="s">
-        <v>221</v>
+        <v>56</v>
       </c>
       <c r="C91">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>57</v>
+        <v>219</v>
       </c>
       <c r="B92" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C92">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>222</v>
+        <v>57</v>
       </c>
       <c r="B93" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C93">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>107</v>
+        <v>221</v>
       </c>
       <c r="B94" t="s">
-        <v>125</v>
+        <v>222</v>
+      </c>
+      <c r="C94">
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B95" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B96" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>110</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>128</v>
+        <v>109</v>
+      </c>
+      <c r="B97" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>111</v>
-      </c>
-      <c r="B98" t="s">
-        <v>129</v>
+        <v>110</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B99" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B100" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B101" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B102" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B103" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B104" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B105" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B106" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B107" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B108" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B109" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B110" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>124</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>141</v>
+        <v>123</v>
+      </c>
+      <c r="B111" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>142</v>
-      </c>
-      <c r="B118" t="s">
-        <v>143</v>
+        <v>164</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B119" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>166</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>203</v>
+        <v>144</v>
+      </c>
+      <c r="B120" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>202</v>
@@ -2326,138 +2647,578 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>146</v>
-      </c>
-      <c r="B123" t="s">
-        <v>176</v>
+        <v>203</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B124" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B125" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B126" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B127" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B128" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B129" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B130" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B131" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B132" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>212</v>
+        <v>175</v>
       </c>
       <c r="B133" t="s">
-        <v>213</v>
+        <v>138</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B134" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>269</v>
+        <v>214</v>
       </c>
       <c r="B135" t="s">
-        <v>270</v>
+        <v>213</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>177</v>
+        <v>268</v>
       </c>
       <c r="B136" t="s">
-        <v>179</v>
+        <v>269</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B137" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>178</v>
+      </c>
+      <c r="B138" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>272</v>
+      </c>
+      <c r="B139" t="s">
         <v>273</v>
       </c>
-      <c r="B138" t="s">
-        <v>274</v>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>276</v>
+      </c>
+      <c r="B140" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>277</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>278</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>279</v>
+      </c>
+      <c r="B143" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>280</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>281</v>
+      </c>
+      <c r="B145" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>282</v>
+      </c>
+      <c r="B146" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>283</v>
+      </c>
+      <c r="B147" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>284</v>
+      </c>
+      <c r="B148" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>295</v>
+      </c>
+      <c r="B149" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>297</v>
+      </c>
+      <c r="B150" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>299</v>
+      </c>
+      <c r="B151" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>301</v>
+      </c>
+      <c r="B152" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>303</v>
+      </c>
+      <c r="B153" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>304</v>
+      </c>
+      <c r="B154" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>305</v>
+      </c>
+      <c r="B155" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>307</v>
+      </c>
+      <c r="B156" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>309</v>
+      </c>
+      <c r="B157" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>311</v>
+      </c>
+      <c r="B158" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>332</v>
+      </c>
+      <c r="B159" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>334</v>
+      </c>
+      <c r="B160" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>313</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>314</v>
+      </c>
+      <c r="B162" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>315</v>
+      </c>
+      <c r="B163" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>316</v>
+      </c>
+      <c r="B164" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>320</v>
+      </c>
+      <c r="B165" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>321</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>322</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>325</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>323</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>324</v>
+      </c>
+      <c r="B170" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>326</v>
+      </c>
+      <c r="B171" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>328</v>
+      </c>
+      <c r="B172" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>329</v>
+      </c>
+      <c r="B173" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>330</v>
+      </c>
+      <c r="B174" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>331</v>
+      </c>
+      <c r="B175" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>336</v>
+      </c>
+      <c r="B176" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>337</v>
+      </c>
+      <c r="B177" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>338</v>
+      </c>
+      <c r="B178" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>340</v>
+      </c>
+      <c r="B179" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>347</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>348</v>
+      </c>
+      <c r="B181" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>349</v>
+      </c>
+      <c r="B182" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>353</v>
+      </c>
+      <c r="B183" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>354</v>
+      </c>
+      <c r="B184" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>355</v>
+      </c>
+      <c r="B185" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>356</v>
+      </c>
+      <c r="B186" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>358</v>
+      </c>
+      <c r="B187" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>359</v>
+      </c>
+      <c r="B188" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>371</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>373</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>376</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>377</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>378</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sfx and music, some fixes and adjustment
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E3626F-7A41-423A-86D5-88E88EFC1AB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3A7A21-13C7-413A-A165-BFCFAB475A6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5130" yWindow="3090" windowWidth="19065" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,15 +418,9 @@
     <t>Septic Water</t>
   </si>
   <si>
-    <t>The kind of water found in sewer where all the wastes accumulate. A perfect home for all sorts of bacteria.</t>
-  </si>
-  <si>
     <t>Pond</t>
   </si>
   <si>
-    <t>Known as the windpipe that connects the larynx, and the bronchi of the lungs. Many foreign organisms are disposed of here by the hands of white blood cells. Beware of the wandering macrophages.</t>
-  </si>
-  <si>
     <t>Trachea</t>
   </si>
   <si>
@@ -439,9 +433,6 @@
     <t>Whirlpool</t>
   </si>
   <si>
-    <t>A body of freshwater within a land brimming with life. Where there are thriving populations of organisms, so too, will there be predators.</t>
-  </si>
-  <si>
     <t>A body of freshwater within a land brimming with life. A perfect place for predatory organisms.</t>
   </si>
   <si>
@@ -1232,6 +1223,15 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>Plenty of wastes to be found here. These waters have become a breeding ground for methanogens.</t>
+  </si>
+  <si>
+    <t>A body of freshwater brimming with life. Water plants provide a good source of energy, and there’s plenty of sunlight.</t>
+  </si>
+  <si>
+    <t>Known as the windpipe that connects the larynx, and the bronchi of the lungs. Many foreign organisms are disposed of here by the hands of white blood cells. Beware the wandering macrophages!</t>
   </si>
 </sst>
 </file>
@@ -1569,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="A203" sqref="A203"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1651,10 +1651,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1851,26 +1851,26 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B33" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B34" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B35" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1918,10 +1918,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B41" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C41">
         <v>8</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B43" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C43">
         <v>8</v>
@@ -1962,10 +1962,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C45">
         <v>8</v>
@@ -1973,10 +1973,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -1984,10 +1984,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B47" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C47">
         <v>8</v>
@@ -1995,10 +1995,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C48">
         <v>3</v>
@@ -2006,10 +2006,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C49">
         <v>8</v>
@@ -2017,10 +2017,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -2028,10 +2028,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B51" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C51">
         <v>8</v>
@@ -2039,10 +2039,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C53">
         <v>8</v>
@@ -2061,10 +2061,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C54">
         <v>2</v>
@@ -2072,10 +2072,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B55" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C55">
         <v>8</v>
@@ -2115,10 +2115,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B60" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C60">
         <v>2</v>
@@ -2126,10 +2126,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B61" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C61">
         <v>8</v>
@@ -2137,10 +2137,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B62" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C62">
         <v>2</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B63" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C63">
         <v>8</v>
@@ -2159,10 +2159,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B64" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C64">
         <v>2</v>
@@ -2170,10 +2170,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C65">
         <v>8</v>
@@ -2192,10 +2192,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B67" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C67">
         <v>8</v>
@@ -2222,10 +2222,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C70">
         <v>8</v>
@@ -2244,10 +2244,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C72">
         <v>8</v>
@@ -2266,10 +2266,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C74">
         <v>8</v>
@@ -2288,10 +2288,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B76" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C76">
         <v>8</v>
@@ -2310,10 +2310,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C78">
         <v>8</v>
@@ -2332,10 +2332,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B80" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C80">
         <v>8</v>
@@ -2343,10 +2343,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B81" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C81">
         <v>2</v>
@@ -2354,10 +2354,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B82" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C82">
         <v>8</v>
@@ -2365,10 +2365,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B83" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C83">
         <v>2</v>
@@ -2376,10 +2376,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B84" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C84">
         <v>8</v>
@@ -2387,10 +2387,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>259</v>
+      </c>
+      <c r="B85" t="s">
         <v>262</v>
-      </c>
-      <c r="B85" t="s">
-        <v>265</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -2398,10 +2398,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B86" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C86">
         <v>8</v>
@@ -2420,10 +2420,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C88">
         <v>8</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B90" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C90">
         <v>8</v>
@@ -2464,10 +2464,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B92" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C92">
         <v>8</v>
@@ -2478,7 +2478,7 @@
         <v>57</v>
       </c>
       <c r="B93" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C93">
         <v>4</v>
@@ -2486,10 +2486,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B94" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C94">
         <v>8</v>
@@ -2556,7 +2556,7 @@
         <v>114</v>
       </c>
       <c r="B102" t="s">
-        <v>132</v>
+        <v>401</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2564,7 +2564,7 @@
         <v>115</v>
       </c>
       <c r="B103" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2572,7 +2572,7 @@
         <v>116</v>
       </c>
       <c r="B104" t="s">
-        <v>139</v>
+        <v>402</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2580,7 +2580,7 @@
         <v>117</v>
       </c>
       <c r="B105" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2588,7 +2588,7 @@
         <v>118</v>
       </c>
       <c r="B106" t="s">
-        <v>134</v>
+        <v>403</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2596,7 +2596,7 @@
         <v>119</v>
       </c>
       <c r="B107" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2604,7 +2604,7 @@
         <v>120</v>
       </c>
       <c r="B108" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2612,7 +2612,7 @@
         <v>121</v>
       </c>
       <c r="B109" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2620,7 +2620,7 @@
         <v>122</v>
       </c>
       <c r="B110" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2628,7 +2628,7 @@
         <v>123</v>
       </c>
       <c r="B111" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2636,396 +2636,396 @@
         <v>124</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B119" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B120" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B124" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B125" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B126" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B127" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B128" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B129" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B130" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B131" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B132" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B133" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B134" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B135" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B136" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B137" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B138" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B139" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B140" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B143" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B145" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B146" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B147" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B148" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B149" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B150" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B151" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B152" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B153" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B154" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B155" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B156" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B157" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B158" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B159" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B160" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>5</v>
@@ -3033,346 +3033,346 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
+        <v>311</v>
+      </c>
+      <c r="B162" t="s">
         <v>314</v>
-      </c>
-      <c r="B162" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>312</v>
+      </c>
+      <c r="B163" t="s">
         <v>315</v>
-      </c>
-      <c r="B163" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>313</v>
+      </c>
+      <c r="B164" t="s">
         <v>316</v>
-      </c>
-      <c r="B164" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B165" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
+        <v>321</v>
+      </c>
+      <c r="B170" t="s">
         <v>324</v>
-      </c>
-      <c r="B170" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B171" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B172" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B173" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B174" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B175" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B176" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B177" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B178" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B179" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>344</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>345</v>
+      </c>
+      <c r="B181" t="s">
         <v>348</v>
-      </c>
-      <c r="B181" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>346</v>
+      </c>
+      <c r="B182" t="s">
         <v>349</v>
-      </c>
-      <c r="B182" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B183" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>351</v>
+      </c>
+      <c r="B184" t="s">
         <v>354</v>
-      </c>
-      <c r="B184" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B185" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B186" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B187" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B188" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>368</v>
+      </c>
+      <c r="B189" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>373</v>
+      </c>
+      <c r="B191" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>374</v>
+      </c>
+      <c r="B192" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>375</v>
+      </c>
+      <c r="B193" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B194" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B195" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>391</v>
+      </c>
+      <c r="B198" t="s">
         <v>394</v>
-      </c>
-      <c r="B198" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>384</v>
+      </c>
+      <c r="B199" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
+        <v>385</v>
+      </c>
+      <c r="B200" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
+        <v>386</v>
+      </c>
+      <c r="B201" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="B201" s="2" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial restructure of categories in archaea
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3A7A21-13C7-413A-A165-BFCFAB475A6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AE7BDB-6863-4D68-92BD-6D610F3EDD9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="3090" windowWidth="19065" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7905" yWindow="3810" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="398">
   <si>
     <t>Key</t>
   </si>
@@ -43,30 +43,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>Test 1</t>
-  </si>
-  <si>
-    <t>Test 2</t>
-  </si>
-  <si>
-    <t>testBodyCapsule</t>
-  </si>
-  <si>
-    <t>Capsule</t>
-  </si>
-  <si>
-    <t>testBodySphere</t>
-  </si>
-  <si>
-    <t>Sphere</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -1232,6 +1208,12 @@
   </si>
   <si>
     <t>Known as the windpipe that connects the larynx, and the bronchi of the lungs. Many foreign organisms are disposed of here by the hands of white blood cells. Beware the wandering macrophages!</t>
+  </si>
+  <si>
+    <t>categoryMembrane</t>
+  </si>
+  <si>
+    <t>Membrane</t>
   </si>
 </sst>
 </file>
@@ -1567,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D204"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,514 +1596,523 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>259</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>267</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>268</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>194</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>196</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>198</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>202</v>
+        <v>396</v>
       </c>
       <c r="B33" t="s">
-        <v>203</v>
+        <v>397</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>204</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>205</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>206</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>207</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>170</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>171</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>13</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>172</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>283</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>178</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>179</v>
+        <v>37</v>
       </c>
       <c r="C41">
-        <v>8</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" t="s">
-        <v>21</v>
+        <v>173</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>180</v>
-      </c>
-      <c r="B43" t="s">
-        <v>291</v>
+        <v>217</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="C43">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>219</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>232</v>
       </c>
       <c r="C44">
-        <v>2.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>220</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>182</v>
+        <v>221</v>
       </c>
       <c r="C45">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>227</v>
-      </c>
-      <c r="B47" t="s">
-        <v>240</v>
+        <v>223</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>224</v>
       </c>
       <c r="C47">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>228</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
+      </c>
+      <c r="B48" t="s">
+        <v>234</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C49">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>233</v>
-      </c>
-      <c r="B51" t="s">
-        <v>242</v>
+        <v>229</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="C51">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>234</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
+      </c>
+      <c r="B52" t="s">
+        <v>236</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>236</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C53">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="B53" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>237</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C54">
-        <v>2</v>
+        <v>33</v>
+      </c>
+      <c r="B54" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>239</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>244</v>
-      </c>
-      <c r="C55">
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>237</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>238</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>239</v>
       </c>
       <c r="B58" t="s">
-        <v>44</v>
+        <v>240</v>
+      </c>
+      <c r="C58">
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>241</v>
       </c>
       <c r="B59" t="s">
-        <v>49</v>
+        <v>243</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B60" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C60">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2132,59 +2123,56 @@
         <v>248</v>
       </c>
       <c r="C61">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>249</v>
-      </c>
-      <c r="B62" t="s">
-        <v>251</v>
+        <v>245</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>250</v>
+        <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>252</v>
+        <v>15</v>
       </c>
       <c r="C63">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>255</v>
+        <v>175</v>
       </c>
       <c r="B64" t="s">
-        <v>256</v>
+        <v>176</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>253</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C65">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C66">
         <v>2</v>
@@ -2192,10 +2180,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>183</v>
-      </c>
-      <c r="B67" t="s">
-        <v>184</v>
+        <v>177</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="C67">
         <v>8</v>
@@ -2203,725 +2191,719 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B68" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>27</v>
-      </c>
-      <c r="B69" t="s">
-        <v>28</v>
+        <v>179</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>185</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>186</v>
+        <v>23</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
       </c>
       <c r="C70">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>29</v>
-      </c>
-      <c r="B71" t="s">
-        <v>30</v>
+        <v>181</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="C71">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>187</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>188</v>
+        <v>25</v>
+      </c>
+      <c r="B72" t="s">
+        <v>26</v>
       </c>
       <c r="C72">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>31</v>
+        <v>182</v>
       </c>
       <c r="B73" t="s">
-        <v>32</v>
+        <v>184</v>
       </c>
       <c r="C73">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>189</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>191</v>
+        <v>27</v>
+      </c>
+      <c r="B74" t="s">
+        <v>28</v>
       </c>
       <c r="C74">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>33</v>
-      </c>
-      <c r="B75" t="s">
-        <v>34</v>
+        <v>186</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="C75">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>190</v>
+        <v>29</v>
       </c>
       <c r="B76" t="s">
-        <v>192</v>
+        <v>30</v>
       </c>
       <c r="C76">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>35</v>
+        <v>187</v>
       </c>
       <c r="B77" t="s">
-        <v>36</v>
+        <v>188</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>194</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>193</v>
+        <v>212</v>
+      </c>
+      <c r="B78" t="s">
+        <v>213</v>
       </c>
       <c r="C78">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>37</v>
+        <v>214</v>
       </c>
       <c r="B79" t="s">
-        <v>38</v>
+        <v>215</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>195</v>
+        <v>249</v>
       </c>
       <c r="B80" t="s">
-        <v>196</v>
+        <v>253</v>
       </c>
       <c r="C80">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="B81" t="s">
-        <v>221</v>
+        <v>255</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>222</v>
+        <v>251</v>
       </c>
       <c r="B82" t="s">
-        <v>223</v>
+        <v>254</v>
       </c>
       <c r="C82">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B83" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C83">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="B84" t="s">
-        <v>263</v>
+        <v>46</v>
       </c>
       <c r="C84">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>259</v>
-      </c>
-      <c r="B85" t="s">
-        <v>262</v>
+        <v>205</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>206</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>260</v>
+        <v>51</v>
       </c>
       <c r="B86" t="s">
-        <v>264</v>
+        <v>52</v>
       </c>
       <c r="C86">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>53</v>
+        <v>207</v>
       </c>
       <c r="B87" t="s">
-        <v>54</v>
+        <v>216</v>
       </c>
       <c r="C87">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>213</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>214</v>
+        <v>47</v>
+      </c>
+      <c r="B88" t="s">
+        <v>48</v>
       </c>
       <c r="C88">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>59</v>
+        <v>208</v>
       </c>
       <c r="B89" t="s">
-        <v>60</v>
+        <v>209</v>
       </c>
       <c r="C89">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>215</v>
+        <v>49</v>
       </c>
       <c r="B90" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="C90">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>55</v>
+        <v>210</v>
       </c>
       <c r="B91" t="s">
-        <v>56</v>
+        <v>211</v>
       </c>
       <c r="C91">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>216</v>
+        <v>99</v>
       </c>
       <c r="B92" t="s">
-        <v>217</v>
-      </c>
-      <c r="C92">
-        <v>8</v>
+        <v>117</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="B93" t="s">
-        <v>212</v>
-      </c>
-      <c r="C93">
-        <v>4</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>218</v>
+        <v>101</v>
       </c>
       <c r="B94" t="s">
-        <v>219</v>
-      </c>
-      <c r="C94">
-        <v>8</v>
+        <v>119</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>107</v>
-      </c>
-      <c r="B95" t="s">
-        <v>125</v>
+        <v>102</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B96" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B97" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>110</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>128</v>
+        <v>105</v>
+      </c>
+      <c r="B98" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B99" t="s">
-        <v>129</v>
+        <v>393</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B100" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B101" t="s">
-        <v>131</v>
+        <v>394</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B102" t="s">
-        <v>401</v>
+        <v>125</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B103" t="s">
-        <v>132</v>
+        <v>395</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B104" t="s">
-        <v>402</v>
+        <v>124</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B105" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B106" t="s">
-        <v>403</v>
+        <v>126</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B107" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B108" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>121</v>
-      </c>
-      <c r="B109" t="s">
-        <v>134</v>
+        <v>116</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>122</v>
-      </c>
-      <c r="B110" t="s">
-        <v>135</v>
+        <v>140</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>123</v>
-      </c>
-      <c r="B111" t="s">
-        <v>136</v>
+        <v>142</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>155</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>154</v>
+        <v>131</v>
+      </c>
+      <c r="B116" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>160</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>157</v>
+        <v>133</v>
+      </c>
+      <c r="B117" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>162</v>
+        <v>191</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>139</v>
-      </c>
-      <c r="B119" t="s">
-        <v>140</v>
+        <v>189</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>141</v>
-      </c>
-      <c r="B120" t="s">
-        <v>142</v>
+        <v>192</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>163</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>199</v>
+        <v>135</v>
+      </c>
+      <c r="B121" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>197</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>198</v>
+        <v>136</v>
+      </c>
+      <c r="B122" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>200</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>201</v>
+        <v>138</v>
+      </c>
+      <c r="B123" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B124" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B125" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B126" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B127" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B128" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B129" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B130" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="B131" t="s">
-        <v>168</v>
+        <v>201</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="B132" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>172</v>
+        <v>257</v>
       </c>
       <c r="B133" t="s">
-        <v>136</v>
+        <v>258</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>208</v>
+        <v>166</v>
       </c>
       <c r="B134" t="s">
-        <v>209</v>
+        <v>168</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>211</v>
+        <v>167</v>
       </c>
       <c r="B135" t="s">
-        <v>210</v>
+        <v>169</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B136" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>174</v>
+        <v>265</v>
       </c>
       <c r="B137" t="s">
-        <v>176</v>
+        <v>282</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>175</v>
-      </c>
-      <c r="B138" t="s">
-        <v>177</v>
+        <v>266</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>269</v>
-      </c>
-      <c r="B139" t="s">
-        <v>270</v>
+        <v>267</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B140" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>275</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>283</v>
+        <v>270</v>
+      </c>
+      <c r="B142" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B143" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>277</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>285</v>
+        <v>272</v>
+      </c>
+      <c r="B144" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B145" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="B146" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B147" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="B148" t="s">
         <v>289</v>
@@ -2929,415 +2911,415 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B149" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B150" t="s">
-        <v>295</v>
+        <v>195</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B151" t="s">
-        <v>297</v>
+        <v>197</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B152" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B153" t="s">
-        <v>203</v>
+        <v>297</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B154" t="s">
-        <v>205</v>
+        <v>299</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B155" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>304</v>
+        <v>321</v>
       </c>
       <c r="B156" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="B157" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>308</v>
-      </c>
-      <c r="B158" t="s">
-        <v>309</v>
+        <v>302</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>329</v>
+        <v>303</v>
       </c>
       <c r="B159" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="B160" t="s">
-        <v>332</v>
+        <v>307</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>310</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>5</v>
+        <v>305</v>
+      </c>
+      <c r="B161" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B162" t="s">
-        <v>314</v>
+        <v>356</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>312</v>
-      </c>
-      <c r="B163" t="s">
-        <v>315</v>
+        <v>310</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>313</v>
-      </c>
-      <c r="B164" t="s">
-        <v>316</v>
+        <v>311</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>317</v>
-      </c>
-      <c r="B165" t="s">
-        <v>364</v>
+        <v>314</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>319</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>366</v>
+        <v>313</v>
+      </c>
+      <c r="B167" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>322</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>367</v>
+        <v>315</v>
+      </c>
+      <c r="B168" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>320</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>369</v>
+        <v>317</v>
+      </c>
+      <c r="B169" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B170" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B171" t="s">
-        <v>359</v>
+        <v>332</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B172" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B173" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B174" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>327</v>
+      </c>
+      <c r="B175" t="s">
         <v>328</v>
-      </c>
-      <c r="B175" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B176" t="s">
-        <v>358</v>
+        <v>335</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>334</v>
-      </c>
-      <c r="B177" t="s">
-        <v>342</v>
+        <v>336</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B178" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B179" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>344</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>347</v>
+        <v>342</v>
+      </c>
+      <c r="B180" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B181" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B182" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B183" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B184" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B185" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>353</v>
-      </c>
-      <c r="B186" t="s">
         <v>360</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>355</v>
-      </c>
-      <c r="B187" t="s">
-        <v>357</v>
+        <v>362</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>356</v>
-      </c>
-      <c r="B188" t="s">
-        <v>363</v>
+        <v>365</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>367</v>
+      </c>
+      <c r="B190" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>373</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>376</v>
+        <v>371</v>
+      </c>
+      <c r="B191" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>374</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>377</v>
+        <v>372</v>
+      </c>
+      <c r="B192" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>379</v>
-      </c>
-      <c r="B194" t="s">
-        <v>390</v>
+        <v>375</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B195" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>391</v>
-      </c>
-      <c r="B198" t="s">
-        <v>394</v>
+        <v>378</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>388</v>
@@ -3345,34 +3327,10 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>400</v>
-      </c>
-      <c r="B202" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>395</v>
-      </c>
-      <c r="B203" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>397</v>
-      </c>
-      <c r="B204" s="2" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
setup separation of membrane and metabolism data for archaea
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AE7BDB-6863-4D68-92BD-6D610F3EDD9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D6D7F1-A969-4CC1-A895-682A51EEEBC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7905" yWindow="3810" windowWidth="22875" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="406">
   <si>
     <t>Key</t>
   </si>
@@ -70,24 +70,12 @@
     <t>Thermophile</t>
   </si>
   <si>
-    <t>cellStructureThermophile</t>
-  </si>
-  <si>
-    <t>cellStructurePsychrophile</t>
-  </si>
-  <si>
-    <t>Psychrophile</t>
-  </si>
-  <si>
     <t>cellStructureMethanogen</t>
   </si>
   <si>
     <t>Methanogen</t>
   </si>
   <si>
-    <t>cellStructureHalophile</t>
-  </si>
-  <si>
     <t>Halophile</t>
   </si>
   <si>
@@ -547,9 +535,6 @@
     <t>These are extra DNA molecules that are commonly found in bacteria, and sometimes in other cells. They allow cells to mutate and adapt to an ever-changing environment.</t>
   </si>
   <si>
-    <t>cellStructureThermophileDesc</t>
-  </si>
-  <si>
     <t>An affinity for extremely hot temperature. These archaeans can thrive in environments near volcanos, hot springs, and acidic soils.</t>
   </si>
   <si>
@@ -559,9 +544,6 @@
     <t>These archaeans release methane as a result of digesting materials such as carbon and hydrogen. They are known to play a role in breaking up materials for other cells to consume.</t>
   </si>
   <si>
-    <t>cellStructureHalophileDesc</t>
-  </si>
-  <si>
     <t>An affinity for salt. These archaeans can withstand the effects of salt which causes dehydration. They are also known to be resistant to UV radiation, giving them a reddish look.</t>
   </si>
   <si>
@@ -1214,6 +1196,48 @@
   </si>
   <si>
     <t>Membrane</t>
+  </si>
+  <si>
+    <t>bodyArchaeaAnaerobe</t>
+  </si>
+  <si>
+    <t>bodyArchaeaAnaerobeDesc</t>
+  </si>
+  <si>
+    <t>Anaerobe</t>
+  </si>
+  <si>
+    <t>&lt;desc&gt;</t>
+  </si>
+  <si>
+    <t>bodyArchaeaHalophile</t>
+  </si>
+  <si>
+    <t>bodyArchaeaHalophileDesc</t>
+  </si>
+  <si>
+    <t>bodyArchaeaThermophile</t>
+  </si>
+  <si>
+    <t>bodyArchaeaThermophileDesc</t>
+  </si>
+  <si>
+    <t>metabolismAminoAcid</t>
+  </si>
+  <si>
+    <t>metabolismAminoAcidDesc</t>
+  </si>
+  <si>
+    <t>metabolismHydrogen</t>
+  </si>
+  <si>
+    <t>metabolismHydrogenDesc</t>
+  </si>
+  <si>
+    <t>metabolismSulfur</t>
+  </si>
+  <si>
+    <t>metabolismSulfurDesc</t>
   </si>
 </sst>
 </file>
@@ -1549,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,15 +1620,15 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1617,210 +1641,210 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B30" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1828,15 +1852,15 @@
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B33" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1844,7 +1868,7 @@
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1857,15 +1881,15 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
@@ -1876,10 +1900,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B38" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C38">
         <v>8</v>
@@ -1887,7 +1911,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
         <v>13</v>
@@ -1898,10 +1922,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B40" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C40">
         <v>8</v>
@@ -1909,10 +1933,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C41">
         <v>2.5</v>
@@ -1920,10 +1944,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C42">
         <v>8</v>
@@ -1931,10 +1955,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -1942,10 +1966,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B44" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C44">
         <v>8</v>
@@ -1953,10 +1977,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C45">
         <v>3</v>
@@ -1964,10 +1988,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C46">
         <v>8</v>
@@ -1975,10 +1999,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C47">
         <v>3</v>
@@ -1986,10 +2010,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B48" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C48">
         <v>8</v>
@@ -1997,10 +2021,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -2008,10 +2032,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C50">
         <v>8</v>
@@ -2019,10 +2043,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -2030,10 +2054,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B52" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C52">
         <v>8</v>
@@ -2041,42 +2065,42 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>237</v>
+        <v>392</v>
       </c>
       <c r="B57" t="s">
-        <v>238</v>
+        <v>394</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -2084,10 +2108,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>239</v>
+        <v>393</v>
       </c>
       <c r="B58" t="s">
-        <v>240</v>
+        <v>395</v>
       </c>
       <c r="C58">
         <v>8</v>
@@ -2095,10 +2119,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>241</v>
+        <v>396</v>
       </c>
       <c r="B59" t="s">
-        <v>243</v>
+        <v>18</v>
       </c>
       <c r="C59">
         <v>2</v>
@@ -2106,10 +2130,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>242</v>
+        <v>397</v>
       </c>
       <c r="B60" t="s">
-        <v>244</v>
+        <v>174</v>
       </c>
       <c r="C60">
         <v>8</v>
@@ -2117,10 +2141,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>247</v>
+        <v>398</v>
       </c>
       <c r="B61" t="s">
-        <v>248</v>
+        <v>15</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -2128,10 +2152,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>245</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>246</v>
+        <v>399</v>
+      </c>
+      <c r="B62" t="s">
+        <v>171</v>
       </c>
       <c r="C62">
         <v>8</v>
@@ -2139,10 +2163,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>16</v>
+        <v>231</v>
       </c>
       <c r="B63" t="s">
-        <v>15</v>
+        <v>232</v>
       </c>
       <c r="C63">
         <v>2</v>
@@ -2150,10 +2174,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>175</v>
+        <v>233</v>
       </c>
       <c r="B64" t="s">
-        <v>176</v>
+        <v>234</v>
       </c>
       <c r="C64">
         <v>8</v>
@@ -2161,1176 +2185,1256 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>235</v>
       </c>
       <c r="B65" t="s">
-        <v>18</v>
+        <v>237</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>236</v>
       </c>
       <c r="B66" t="s">
-        <v>20</v>
+        <v>238</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>177</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>178</v>
+        <v>241</v>
+      </c>
+      <c r="B67" t="s">
+        <v>242</v>
       </c>
       <c r="C67">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>21</v>
-      </c>
-      <c r="B68" t="s">
-        <v>22</v>
+        <v>239</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>179</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>180</v>
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>17</v>
       </c>
       <c r="C69">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70" t="s">
-        <v>24</v>
+        <v>172</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="C70">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>181</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>183</v>
+        <v>19</v>
+      </c>
+      <c r="B71" t="s">
+        <v>20</v>
       </c>
       <c r="C71">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>25</v>
-      </c>
-      <c r="B72" t="s">
-        <v>26</v>
+        <v>175</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>182</v>
+        <v>21</v>
       </c>
       <c r="B73" t="s">
-        <v>184</v>
+        <v>22</v>
       </c>
       <c r="C73">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>176</v>
       </c>
       <c r="B74" t="s">
-        <v>28</v>
+        <v>178</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>186</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>185</v>
+        <v>23</v>
+      </c>
+      <c r="B75" t="s">
+        <v>24</v>
       </c>
       <c r="C75">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>29</v>
-      </c>
-      <c r="B76" t="s">
-        <v>30</v>
+        <v>180</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="C76">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>187</v>
+        <v>25</v>
       </c>
       <c r="B77" t="s">
-        <v>188</v>
+        <v>26</v>
       </c>
       <c r="C77">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="B78" t="s">
-        <v>213</v>
+        <v>182</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B79" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C79">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>249</v>
+        <v>208</v>
       </c>
       <c r="B80" t="s">
-        <v>253</v>
+        <v>209</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="B81" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C81">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B82" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B83" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C83">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>45</v>
+        <v>246</v>
       </c>
       <c r="B84" t="s">
-        <v>46</v>
+        <v>250</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>205</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>206</v>
+        <v>400</v>
+      </c>
+      <c r="B85" t="s">
+        <v>141</v>
       </c>
       <c r="C85">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>51</v>
+        <v>401</v>
       </c>
       <c r="B86" t="s">
-        <v>52</v>
+        <v>395</v>
       </c>
       <c r="C86">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>207</v>
+        <v>402</v>
       </c>
       <c r="B87" t="s">
-        <v>216</v>
+        <v>139</v>
       </c>
       <c r="C87">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>47</v>
+        <v>403</v>
       </c>
       <c r="B88" t="s">
-        <v>48</v>
+        <v>395</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>208</v>
+        <v>404</v>
       </c>
       <c r="B89" t="s">
-        <v>209</v>
+        <v>137</v>
       </c>
       <c r="C89">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>49</v>
+        <v>405</v>
       </c>
       <c r="B90" t="s">
-        <v>204</v>
+        <v>395</v>
       </c>
       <c r="C90">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>210</v>
+        <v>41</v>
       </c>
       <c r="B91" t="s">
-        <v>211</v>
+        <v>42</v>
       </c>
       <c r="C91">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>99</v>
-      </c>
-      <c r="B92" t="s">
-        <v>117</v>
+        <v>199</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C92">
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="B93" t="s">
-        <v>118</v>
+        <v>48</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>101</v>
+        <v>201</v>
       </c>
       <c r="B94" t="s">
-        <v>119</v>
+        <v>210</v>
+      </c>
+      <c r="C94">
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>102</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>120</v>
+        <v>43</v>
+      </c>
+      <c r="B95" t="s">
+        <v>44</v>
+      </c>
+      <c r="C95">
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>202</v>
+      </c>
+      <c r="B96" t="s">
+        <v>203</v>
+      </c>
+      <c r="C96">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>45</v>
+      </c>
+      <c r="B97" t="s">
+        <v>198</v>
+      </c>
+      <c r="C97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>204</v>
+      </c>
+      <c r="B98" t="s">
+        <v>205</v>
+      </c>
+      <c r="C98">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>95</v>
+      </c>
+      <c r="B99" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>96</v>
+      </c>
+      <c r="B100" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>97</v>
+      </c>
+      <c r="B101" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>98</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>99</v>
+      </c>
+      <c r="B103" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>100</v>
+      </c>
+      <c r="B104" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>101</v>
+      </c>
+      <c r="B105" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>102</v>
+      </c>
+      <c r="B106" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>103</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B107" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>104</v>
+      </c>
+      <c r="B108" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>105</v>
+      </c>
+      <c r="B109" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>104</v>
-      </c>
-      <c r="B97" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>105</v>
-      </c>
-      <c r="B98" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>106</v>
       </c>
-      <c r="B99" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="B110" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>107</v>
       </c>
-      <c r="B100" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="B111" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>108</v>
       </c>
-      <c r="B101" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>109</v>
-      </c>
-      <c r="B102" t="s">
+      <c r="B112" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>110</v>
-      </c>
-      <c r="B103" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>111</v>
-      </c>
-      <c r="B104" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>112</v>
-      </c>
-      <c r="B105" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>113</v>
-      </c>
-      <c r="B106" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>114</v>
-      </c>
-      <c r="B107" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>115</v>
-      </c>
-      <c r="B108" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>116</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>140</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>142</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>144</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>147</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>146</v>
+        <v>109</v>
+      </c>
+      <c r="B113" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>152</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>149</v>
+        <v>110</v>
+      </c>
+      <c r="B114" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>153</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>154</v>
+        <v>111</v>
+      </c>
+      <c r="B115" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>131</v>
-      </c>
-      <c r="B116" t="s">
-        <v>132</v>
+        <v>112</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>133</v>
-      </c>
-      <c r="B117" t="s">
-        <v>134</v>
+        <v>136</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>192</v>
+        <v>143</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>193</v>
+        <v>142</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>135</v>
-      </c>
-      <c r="B121" t="s">
-        <v>165</v>
+        <v>148</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>136</v>
-      </c>
-      <c r="B122" t="s">
-        <v>137</v>
+        <v>149</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B123" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B124" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>150</v>
-      </c>
-      <c r="B125" t="s">
         <v>151</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>156</v>
-      </c>
-      <c r="B126" t="s">
-        <v>161</v>
+        <v>183</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>157</v>
-      </c>
-      <c r="B127" t="s">
-        <v>158</v>
+        <v>186</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="B128" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="B129" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="B130" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>200</v>
+        <v>144</v>
       </c>
       <c r="B131" t="s">
-        <v>201</v>
+        <v>145</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>203</v>
+        <v>146</v>
       </c>
       <c r="B132" t="s">
-        <v>202</v>
+        <v>147</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>257</v>
+        <v>152</v>
       </c>
       <c r="B133" t="s">
-        <v>258</v>
+        <v>157</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="B134" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B135" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>261</v>
+        <v>158</v>
       </c>
       <c r="B136" t="s">
-        <v>262</v>
+        <v>159</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>265</v>
+        <v>160</v>
       </c>
       <c r="B137" t="s">
-        <v>282</v>
+        <v>124</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>266</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>274</v>
+        <v>194</v>
+      </c>
+      <c r="B138" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>267</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>275</v>
+        <v>197</v>
+      </c>
+      <c r="B139" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="B140" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>269</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>277</v>
+        <v>162</v>
+      </c>
+      <c r="B141" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>270</v>
+        <v>163</v>
       </c>
       <c r="B142" t="s">
-        <v>278</v>
+        <v>165</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="B143" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="B144" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>273</v>
-      </c>
-      <c r="B145" t="s">
-        <v>281</v>
+        <v>260</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>284</v>
-      </c>
-      <c r="B146" t="s">
-        <v>285</v>
+        <v>261</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
       <c r="B147" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>288</v>
-      </c>
-      <c r="B148" t="s">
-        <v>289</v>
+        <v>263</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="B149" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
       <c r="B150" t="s">
-        <v>195</v>
+        <v>273</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>293</v>
+        <v>266</v>
       </c>
       <c r="B151" t="s">
-        <v>197</v>
+        <v>274</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="B152" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="B153" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="B154" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="B155" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>321</v>
+        <v>284</v>
       </c>
       <c r="B156" t="s">
-        <v>322</v>
+        <v>285</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>323</v>
+        <v>286</v>
       </c>
       <c r="B157" t="s">
-        <v>324</v>
+        <v>189</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>302</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>5</v>
+        <v>287</v>
+      </c>
+      <c r="B158" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="B159" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="B160" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="B161" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="B162" t="s">
-        <v>356</v>
+        <v>295</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>310</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>357</v>
+        <v>315</v>
+      </c>
+      <c r="B163" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>311</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>358</v>
+        <v>317</v>
+      </c>
+      <c r="B164" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>359</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>312</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>361</v>
+        <v>297</v>
+      </c>
+      <c r="B166" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="B167" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="B168" t="s">
-        <v>351</v>
+        <v>302</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="B169" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>318</v>
-      </c>
-      <c r="B170" t="s">
-        <v>331</v>
+        <v>304</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>319</v>
-      </c>
-      <c r="B171" t="s">
-        <v>332</v>
+        <v>305</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>320</v>
-      </c>
-      <c r="B172" t="s">
-        <v>333</v>
+        <v>308</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>325</v>
-      </c>
-      <c r="B173" t="s">
-        <v>350</v>
+        <v>306</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="B174" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="B175" t="s">
-        <v>328</v>
+        <v>345</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="B176" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>336</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>339</v>
+        <v>312</v>
+      </c>
+      <c r="B177" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="B178" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="B179" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="B180" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>343</v>
+        <v>320</v>
       </c>
       <c r="B181" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>344</v>
+        <v>321</v>
       </c>
       <c r="B182" t="s">
-        <v>353</v>
+        <v>322</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
       <c r="B183" t="s">
-        <v>352</v>
+        <v>329</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>347</v>
-      </c>
-      <c r="B184" t="s">
-        <v>349</v>
+        <v>330</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="B185" t="s">
-        <v>355</v>
+        <v>334</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>360</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>363</v>
+        <v>332</v>
+      </c>
+      <c r="B186" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>362</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>364</v>
+        <v>336</v>
+      </c>
+      <c r="B187" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>365</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>368</v>
+        <v>337</v>
+      </c>
+      <c r="B188" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>366</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>369</v>
+        <v>338</v>
+      </c>
+      <c r="B189" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>367</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>370</v>
+        <v>339</v>
+      </c>
+      <c r="B190" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>371</v>
+        <v>341</v>
       </c>
       <c r="B191" t="s">
-        <v>382</v>
+        <v>343</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>372</v>
+        <v>342</v>
       </c>
       <c r="B192" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>384</v>
+        <v>357</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>385</v>
+        <v>358</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>383</v>
-      </c>
-      <c r="B195" t="s">
-        <v>386</v>
+        <v>359</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>378</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>381</v>
+        <v>365</v>
+      </c>
+      <c r="B198" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>392</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>391</v>
+        <v>366</v>
+      </c>
+      <c r="B199" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>387</v>
+        <v>368</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>390</v>
+        <v>379</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>377</v>
+      </c>
+      <c r="B202" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>370</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>371</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>372</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>386</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>381</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>383</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>